<commit_message>
Aggregated small model updates
</commit_message>
<xml_diff>
--- a/DCF Models/ADI.xlsx
+++ b/DCF Models/ADI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\DCF Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C96F27C-5CC0-4EDB-8F71-7D65E0674B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485C9A43-7F77-4E26-93E0-EC10C9973186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-645" yWindow="4770" windowWidth="32700" windowHeight="15045" activeTab="1" xr2:uid="{2EC0F4CB-CC56-4207-8108-7C832533A8D8}"/>
+    <workbookView xWindow="12360" yWindow="5745" windowWidth="27045" windowHeight="15045" xr2:uid="{2EC0F4CB-CC56-4207-8108-7C832533A8D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
   <si>
     <t>Price</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>Interest on netcash</t>
+  </si>
+  <si>
+    <t>Our IC products are fabricated on proprietary processes at our internal production facilities in Wilmington, Massachusetts; Camas, Washington; Beaverton, Oregon; and Limerick, Ireland and also on a mix of proprietary and nonproprietary processes at third-party wafer fabricators. We currently source more than half of our wafer requirements annually from third-party wafer fabrication foundries, such as Taiwan Semiconductor Manufacturing Company (TSMC) and others, and the remainder is sourced internally</t>
+  </si>
+  <si>
+    <t>we’ve invested $760 million in CapEx to enhance the resiliency of our internal semiconductor manufacturing operations. These investments not only increase our operational resiliency, but also modernize our fabs to better address our sustainability ambitions.</t>
   </si>
 </sst>
 </file>
@@ -261,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -285,6 +291,9 @@
     <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550DD50C-C6AD-42B7-B8F2-B9DA58381265}">
-  <dimension ref="M1:N14"/>
+  <dimension ref="B1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R38" sqref="R38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,7 +775,7 @@
     <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="M1" t="s">
         <v>42</v>
       </c>
@@ -774,17 +783,61 @@
         <v>44980</v>
       </c>
     </row>
-    <row r="3" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
       <c r="M3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
       <c r="M4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
       <c r="M5" t="s">
         <v>0</v>
       </c>
@@ -792,7 +845,17 @@
         <v>185.65</v>
       </c>
     </row>
-    <row r="6" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
       <c r="M6" t="s">
         <v>1</v>
       </c>
@@ -801,7 +864,17 @@
         <v>507.12</v>
       </c>
     </row>
-    <row r="7" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
       <c r="M7" t="s">
         <v>2</v>
       </c>
@@ -810,7 +883,17 @@
         <v>94146.828000000009</v>
       </c>
     </row>
-    <row r="8" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
       <c r="M8" t="s">
         <v>3</v>
       </c>
@@ -818,7 +901,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="9" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="M9" t="s">
         <v>4</v>
       </c>
@@ -827,7 +910,19 @@
         <v>7078</v>
       </c>
     </row>
-    <row r="10" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
       <c r="M10" t="s">
         <v>5</v>
       </c>
@@ -836,7 +931,31 @@
         <v>99554.828000000009</v>
       </c>
     </row>
-    <row r="13" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="M13" t="s">
         <v>38</v>
       </c>
@@ -845,7 +964,7 @@
         <v>95545.612738294119</v>
       </c>
     </row>
-    <row r="14" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="M14" t="s">
         <v>54</v>
       </c>
@@ -855,6 +974,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:K8"/>
+    <mergeCell ref="B10:K12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -864,7 +987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430C4823-B1D5-4075-A061-9C811CDAD08D}">
   <dimension ref="A1:HJ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="J18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1370,7 +1493,7 @@
         <v>18227.740343670008</v>
       </c>
       <c r="AC3" s="4">
-        <f t="shared" ref="Z3:AH3" si="0">AB3*(1+AC39)</f>
+        <f t="shared" ref="AC3:AH3" si="0">AB3*(1+AC39)</f>
         <v>19685.95957116361</v>
       </c>
       <c r="AD3" s="4">

</xml_diff>